<commit_message>
update combined memory usage
</commit_message>
<xml_diff>
--- a/Jimmy-NonImgToImg-code/2022_FFT_benchmarks.xlsx
+++ b/Jimmy-NonImgToImg-code/2022_FFT_benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmyliu/Documents/University/2021/INFO4001/git_repo/Jimmy-nonImageData-Image/Jimmy-NonImgToImg-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F483ACF-3C2E-684C-BB6D-3A9FC2F9F69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563ACDAB-3832-FF44-911C-8375CC0C8367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="deng_reads" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="100">
   <si>
     <t>Dataset</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>3511.99 MiB</t>
+  </si>
+  <si>
+    <t>MemUsed</t>
+  </si>
+  <si>
+    <t>5518.27MiB</t>
+  </si>
+  <si>
+    <t>5546.27 MiB</t>
   </si>
 </sst>
 </file>
@@ -4349,15 +4358,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685D8DF7-8BCA-884D-A2BF-A3097AA67BB7}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4394,8 +4403,11 @@
       <c r="L1" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -4432,8 +4444,11 @@
       <c r="L2" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4470,8 +4485,11 @@
       <c r="L3" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="I4" s="8"/>
     </row>
   </sheetData>
@@ -8212,7 +8230,7 @@
   </sheetPr>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
combined, knn rf, svm
</commit_message>
<xml_diff>
--- a/Jimmy-NonImgToImg-code/2022_FFT_benchmarks.xlsx
+++ b/Jimmy-NonImgToImg-code/2022_FFT_benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmyliu/Documents/University/2021/INFO4001/git_repo/Jimmy-nonImageData-Image/Jimmy-NonImgToImg-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563ACDAB-3832-FF44-911C-8375CC0C8367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EAB14-4806-7A43-BF99-3D4BEDFBE9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="101">
   <si>
     <t>Dataset</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>5546.27 MiB</t>
+  </si>
+  <si>
+    <t>RAW</t>
   </si>
 </sst>
 </file>
@@ -4358,10 +4361,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685D8DF7-8BCA-884D-A2BF-A3097AA67BB7}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4490,7 +4493,112 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="I4" s="8"/>
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>9589</v>
+      </c>
+      <c r="C4">
+        <v>2397</v>
+      </c>
+      <c r="D4">
+        <v>23433</v>
+      </c>
+      <c r="E4">
+        <v>120</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.44169999999999998</v>
+      </c>
+      <c r="K4">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>9589</v>
+      </c>
+      <c r="C5">
+        <v>2397</v>
+      </c>
+      <c r="D5">
+        <v>23433</v>
+      </c>
+      <c r="E5">
+        <v>120</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.67420000000000002</v>
+      </c>
+      <c r="I5">
+        <v>0.67420000000000002</v>
+      </c>
+      <c r="J5">
+        <v>0.3044</v>
+      </c>
+      <c r="K5">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>9589</v>
+      </c>
+      <c r="C6">
+        <v>2397</v>
+      </c>
+      <c r="D6">
+        <v>23433</v>
+      </c>
+      <c r="E6">
+        <v>120</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.32129999999999997</v>
+      </c>
+      <c r="I6">
+        <v>0.32129999999999997</v>
+      </c>
+      <c r="J6">
+        <v>0.04</v>
+      </c>
+      <c r="K6">
+        <v>0.18970000000000001</v>
+      </c>
+      <c r="L6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>